<commit_message>
changed the values of tShape
</commit_message>
<xml_diff>
--- a/Tetris - Grid y Square.xlsx
+++ b/Tetris - Grid y Square.xlsx
@@ -625,7 +625,7 @@
   <dimension ref="A2:AU21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AK10" sqref="AK10"/>
+      <selection activeCell="AA10" sqref="AA10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1298,7 +1298,7 @@
       <c r="V10" s="6">
         <v>0</v>
       </c>
-      <c r="W10" s="11">
+      <c r="W10" s="6">
         <v>1</v>
       </c>
       <c r="X10" s="6">
@@ -1307,7 +1307,7 @@
       <c r="Z10" s="6">
         <v>0</v>
       </c>
-      <c r="AA10" s="6">
+      <c r="AA10" s="11">
         <v>1</v>
       </c>
       <c r="AB10" s="6">
@@ -1389,7 +1389,7 @@
       <c r="W11" s="11">
         <v>11</v>
       </c>
-      <c r="X11" s="6">
+      <c r="X11" s="11">
         <v>12</v>
       </c>
       <c r="Z11" s="11">
@@ -1398,7 +1398,7 @@
       <c r="AA11" s="11">
         <v>11</v>
       </c>
-      <c r="AB11" s="11">
+      <c r="AB11" s="6">
         <v>12</v>
       </c>
       <c r="AE11" s="2"/>

</xml_diff>